<commit_message>
update cash and salary
update exports salary cash with excel (.xlsx)
</commit_message>
<xml_diff>
--- a/Kimeco_ASP/App_Data/templates/SiteCost_Template.xlsx
+++ b/Kimeco_ASP/App_Data/templates/SiteCost_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\GitHub\Kimeco\Kimeco_ASP\App_Data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7746E75-E1D2-418C-B2BA-2A9895A7E4EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7695F69C-2876-45D0-9A5B-1567E531D415}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="8130" xr2:uid="{CC7BD222-957C-467D-8F9A-27FA6A94D16C}"/>
   </bookViews>
@@ -184,9 +184,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -201,6 +198,9 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -797,7 +797,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -815,18 +815,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
@@ -861,84 +861,84 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="4"/>
+      <c r="A3" s="3"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="8"/>
+      <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="A4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="7"/>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="A5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="A6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="7"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="A7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="7"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="A8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="7"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="A9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="8"/>
-      <c r="J10" s="8"/>
+      <c r="A10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="7"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="4"/>
+      <c r="A11" s="3"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="8"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="8"/>
+      <c r="J11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>